<commit_message>
Fix loading systems and improve modal UX
- Fix ChessRecall by removing unnecessary loading system
- Fix HandTask loading system to prevent staggered image/point display
- Implement About acknowledgment with localStorage persistence
- Add About acknowledgment check before app start
- Remove redundant liability and impressum sections from About
- Remove X close buttons from all modal headers
- Add close button to TaskExamples modal for consistency
</commit_message>
<xml_diff>
--- a/GIT Version.xlsx
+++ b/GIT Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areim\Documents\WEBAPPS\distractor-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A314D7BD-2C48-4B76-A2E1-D1579D371874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA836A2-52FE-463E-8F7F-3912748664D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="840" windowWidth="21735" windowHeight="14640" xr2:uid="{52E9E515-A856-4913-8076-17DA4FA96A63}"/>
   </bookViews>
@@ -36,29 +36,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <r>
-      <t>06e1c41</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
+    <t>19.40</t>
   </si>
   <si>
-    <t>19.40</t>
+    <t>bd4e16c</t>
+  </si>
+  <si>
+    <t>06e1c41 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,11 +70,6 @@
       <sz val="14"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,11 +92,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,27 +432,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BEAAB03-D1B3-4B4E-99FF-44A3536525FE}">
-  <dimension ref="B7:D7"/>
+  <dimension ref="B7:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:4" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>46075</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>46079</v>
+      </c>
+      <c r="C8" s="4">
+        <v>51471</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance math task input handling and focus management
- Improve iOS keyboard focus handling in MathTask component
- Add comprehensive input focus management with refs
- Implement iOS-specific overlay for better touch interaction
- Add improved input validation and numeric-only input
- Create inline math task integration in PieTask component
- Add MathTaskModal component for reusable math interactions
- Enhance mobile responsiveness and touch handling
- Update input styling and user experience improvements
</commit_message>
<xml_diff>
--- a/GIT Version.xlsx
+++ b/GIT Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areim\Documents\WEBAPPS\distractor-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA836A2-52FE-463E-8F7F-3912748664D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F4A98D-EA01-4EB0-A9C9-5E329EDEAE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="840" windowWidth="21735" windowHeight="14640" xr2:uid="{52E9E515-A856-4913-8076-17DA4FA96A63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>19.40</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>06e1c41 </t>
+  </si>
+  <si>
+    <t>f6927c0</t>
+  </si>
+  <si>
+    <t>14.06</t>
+  </si>
+  <si>
+    <t>11.50</t>
+  </si>
+  <si>
+    <t>19.52</t>
+  </si>
+  <si>
+    <t>320851d</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -432,16 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BEAAB03-D1B3-4B4E-99FF-44A3536525FE}">
-  <dimension ref="B7:D8"/>
+  <dimension ref="B7:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="4"/>
     <col min="4" max="4" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -449,7 +464,7 @@
       <c r="B7" s="3">
         <v>46075</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -460,11 +475,33 @@
       <c r="B8" s="3">
         <v>46079</v>
       </c>
-      <c r="C8" s="4">
-        <v>51471</v>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>46079</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>46079</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>